<commit_message>
changes on template file
</commit_message>
<xml_diff>
--- a/frontend/src/assets/RFQ_Excel_Template.xlsx
+++ b/frontend/src/assets/RFQ_Excel_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GANESH\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B957EB3C-222D-40E3-8A83-33BDB941A6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7001DA8F-ECC4-4445-8632-212A729949D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F0BB8116-C5C3-48A9-996B-546658BCE51F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F0BB8116-C5C3-48A9-996B-546658BCE51F}"/>
   </bookViews>
   <sheets>
     <sheet name="MPD" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EO!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">INHOUSE!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MPD!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MPD!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,15 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>TASK NO</t>
   </si>
   <si>
     <t>TASK DESCRIPTION</t>
-  </si>
-  <si>
-    <t>11 DIGITS</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
@@ -573,37 +570,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C26E99-9AFB-446A-AE98-595347F933A1}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="29.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
@@ -628,9 +624,6 @@
       </c>
       <c r="K1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -647,18 +640,18 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.26953125" customWidth="1"/>
+    <col min="2" max="2" width="60.54296875" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="37.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,16 +660,16 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -702,17 +695,17 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.26953125" customWidth="1"/>
+    <col min="2" max="2" width="60.54296875" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,13 +714,13 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes on mandatory field and exaple template
</commit_message>
<xml_diff>
--- a/frontend/src/assets/RFQ_Excel_Template.xlsx
+++ b/frontend/src/assets/RFQ_Excel_Template.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">TASK NUMBER</t>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACCESS</t>
   </si>
   <si>
     <t xml:space="preserve">FINAL MH</t>
@@ -330,22 +327,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.73"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="12.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16378" style="0" width="12.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16377" style="0" width="12.8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -354,9 +350,6 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>